<commit_message>
feat: UI top app bar shows “Login as …”; update views, controllers, and migrations
</commit_message>
<xml_diff>
--- a/public/assets/ECSandBackup_Template_AutoCalculation_v1.250804 (UPDATE FORMULA).xlsx
+++ b/public/assets/ECSandBackup_Template_AutoCalculation_v1.250804 (UPDATE FORMULA).xlsx
@@ -159,7 +159,7 @@
     <t xml:space="preserve">Estimated Storage Incremental Backup (GB)</t>
   </si>
   <si>
-    <t xml:space="preserve">CSBS Required?</t>
+    <t xml:space="preserve">CSBS Replication Required?</t>
   </si>
   <si>
     <t xml:space="preserve">Total Replication Copy Retained Second Site</t>
@@ -361,8 +361,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -601,7 +602,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -889,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:AU1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL4" activeCellId="0" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -914,7 +915,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="51.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="38.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="55.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="52.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="29.66"/>
@@ -1255,9 +1256,9 @@
       </c>
       <c r="AJ4" s="14"/>
       <c r="AK4" s="17"/>
-      <c r="AL4" s="18" t="n">
-        <f aca="false">IF(AK4="Yes", R4, 0)</f>
-        <v>0</v>
+      <c r="AL4" s="18" t="e">
+        <f aca="false">IF(at4k4="Yes", R4, 0)</f>
+        <v>#NAME?</v>
       </c>
       <c r="AM4" s="14"/>
       <c r="AN4" s="14"/>

</xml_diff>